<commit_message>
New data and update of parameters
</commit_message>
<xml_diff>
--- a/Folkhalsomyndigheten_Covid19.xlsx
+++ b/Folkhalsomyndigheten_Covid19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="7188" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8610" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 24 May 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 28 May 2020" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -221,10 +221,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,13 +506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W112"/>
+  <dimension ref="A1:W117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -6340,7 +6344,7 @@
         <v>43946</v>
       </c>
       <c r="B83" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -6349,7 +6353,7 @@
         <v>45</v>
       </c>
       <c r="E83" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" s="2">
         <v>23</v>
@@ -6695,7 +6699,7 @@
         <v>43951</v>
       </c>
       <c r="B88" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C88" s="2">
         <v>0</v>
@@ -6728,7 +6732,7 @@
         <v>9</v>
       </c>
       <c r="M88" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N88" s="2">
         <v>176</v>
@@ -7831,7 +7835,7 @@
         <v>43967</v>
       </c>
       <c r="B104" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C104" s="2">
         <v>2</v>
@@ -7867,7 +7871,7 @@
         <v>21</v>
       </c>
       <c r="N104" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O104" s="2">
         <v>5</v>
@@ -8044,7 +8048,7 @@
         <v>43970</v>
       </c>
       <c r="B107" s="2">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C107" s="2">
         <v>6</v>
@@ -8077,7 +8081,7 @@
         <v>2</v>
       </c>
       <c r="M107" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N107" s="2">
         <v>129</v>
@@ -8092,7 +8096,7 @@
         <v>15</v>
       </c>
       <c r="R107" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S107" s="2">
         <v>38</v>
@@ -8115,7 +8119,7 @@
         <v>43971</v>
       </c>
       <c r="B108" s="2">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C108" s="2">
         <v>23</v>
@@ -8133,7 +8137,7 @@
         <v>42</v>
       </c>
       <c r="H108" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I108" s="2">
         <v>32</v>
@@ -8148,10 +8152,10 @@
         <v>7</v>
       </c>
       <c r="M108" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N108" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O108" s="2">
         <v>22</v>
@@ -8163,7 +8167,7 @@
         <v>16</v>
       </c>
       <c r="R108" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S108" s="2">
         <v>27</v>
@@ -8186,7 +8190,7 @@
         <v>43972</v>
       </c>
       <c r="B109" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
@@ -8219,16 +8223,16 @@
         <v>6</v>
       </c>
       <c r="M109" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N109" s="2">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O109" s="2">
         <v>6</v>
       </c>
       <c r="P109" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q109" s="2">
         <v>20</v>
@@ -8240,7 +8244,7 @@
         <v>16</v>
       </c>
       <c r="T109" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U109" s="2">
         <v>168</v>
@@ -8257,7 +8261,7 @@
         <v>43973</v>
       </c>
       <c r="B110" s="2">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C110" s="2">
         <v>10</v>
@@ -8290,16 +8294,16 @@
         <v>3</v>
       </c>
       <c r="M110" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N110" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O110" s="2">
         <v>10</v>
       </c>
       <c r="P110" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q110" s="2">
         <v>2</v>
@@ -8314,7 +8318,7 @@
         <v>11</v>
       </c>
       <c r="U110" s="2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="V110" s="2">
         <v>10</v>
@@ -8328,16 +8332,16 @@
         <v>43974</v>
       </c>
       <c r="B111" s="2">
-        <v>247</v>
+        <v>403</v>
       </c>
       <c r="C111" s="2">
         <v>2</v>
       </c>
       <c r="D111" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E111" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" s="2">
         <v>22</v>
@@ -8346,52 +8350,52 @@
         <v>6</v>
       </c>
       <c r="H111" s="2">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I111" s="2">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="J111" s="2">
         <v>0</v>
       </c>
       <c r="K111" s="2">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="L111" s="2">
         <v>1</v>
       </c>
       <c r="M111" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N111" s="2">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="O111" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P111" s="2">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="Q111" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R111" s="2">
         <v>6</v>
       </c>
       <c r="S111" s="2">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="T111" s="2">
         <v>0</v>
       </c>
       <c r="U111" s="2">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="V111" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W111" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" spans="1:23">
@@ -8399,71 +8403,358 @@
         <v>43975</v>
       </c>
       <c r="B112" s="2">
+        <v>210</v>
+      </c>
+      <c r="C112" s="2">
+        <v>3</v>
+      </c>
+      <c r="D112" s="2">
+        <v>7</v>
+      </c>
+      <c r="E112" s="2">
+        <v>1</v>
+      </c>
+      <c r="F112" s="2">
+        <v>8</v>
+      </c>
+      <c r="G112" s="2">
+        <v>2</v>
+      </c>
+      <c r="H112" s="2">
+        <v>2</v>
+      </c>
+      <c r="I112" s="2">
+        <v>17</v>
+      </c>
+      <c r="J112" s="2">
+        <v>0</v>
+      </c>
+      <c r="K112" s="2">
+        <v>11</v>
+      </c>
+      <c r="L112" s="2">
+        <v>0</v>
+      </c>
+      <c r="M112" s="2">
+        <v>9</v>
+      </c>
+      <c r="N112" s="2">
+        <v>59</v>
+      </c>
+      <c r="O112" s="2">
+        <v>1</v>
+      </c>
+      <c r="P112" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q112" s="2">
+        <v>3</v>
+      </c>
+      <c r="R112" s="2">
+        <v>3</v>
+      </c>
+      <c r="S112" s="2">
+        <v>10</v>
+      </c>
+      <c r="T112" s="2">
+        <v>0</v>
+      </c>
+      <c r="U112" s="2">
+        <v>27</v>
+      </c>
+      <c r="V112" s="2">
+        <v>29</v>
+      </c>
+      <c r="W112" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23">
+      <c r="A113" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B113" s="2">
+        <v>454</v>
+      </c>
+      <c r="C113" s="2">
+        <v>3</v>
+      </c>
+      <c r="D113" s="2">
+        <v>3</v>
+      </c>
+      <c r="E113" s="2">
+        <v>0</v>
+      </c>
+      <c r="F113" s="2">
+        <v>18</v>
+      </c>
+      <c r="G113" s="2">
+        <v>8</v>
+      </c>
+      <c r="H113" s="2">
+        <v>2</v>
+      </c>
+      <c r="I113" s="2">
+        <v>24</v>
+      </c>
+      <c r="J113" s="2">
+        <v>16</v>
+      </c>
+      <c r="K113" s="2">
+        <v>8</v>
+      </c>
+      <c r="L113" s="2">
+        <v>9</v>
+      </c>
+      <c r="M113" s="2">
+        <v>29</v>
+      </c>
+      <c r="N113" s="2">
+        <v>130</v>
+      </c>
+      <c r="O113" s="2">
+        <v>14</v>
+      </c>
+      <c r="P113" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q113" s="2">
+        <v>2</v>
+      </c>
+      <c r="R113" s="2">
+        <v>0</v>
+      </c>
+      <c r="S113" s="2">
+        <v>3</v>
+      </c>
+      <c r="T113" s="2">
+        <v>28</v>
+      </c>
+      <c r="U113" s="2">
+        <v>107</v>
+      </c>
+      <c r="V113" s="2">
+        <v>11</v>
+      </c>
+      <c r="W113" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23">
+      <c r="A114" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B114" s="2">
+        <v>690</v>
+      </c>
+      <c r="C114" s="2">
+        <v>12</v>
+      </c>
+      <c r="D114" s="2">
+        <v>18</v>
+      </c>
+      <c r="E114" s="2">
+        <v>0</v>
+      </c>
+      <c r="F114" s="2">
+        <v>22</v>
+      </c>
+      <c r="G114" s="2">
+        <v>21</v>
+      </c>
+      <c r="H114" s="2">
+        <v>15</v>
+      </c>
+      <c r="I114" s="2">
+        <v>35</v>
+      </c>
+      <c r="J114" s="2">
+        <v>17</v>
+      </c>
+      <c r="K114" s="2">
+        <v>12</v>
+      </c>
+      <c r="L114" s="2">
+        <v>7</v>
+      </c>
+      <c r="M114" s="2">
+        <v>51</v>
+      </c>
+      <c r="N114" s="2">
+        <v>146</v>
+      </c>
+      <c r="O114" s="2">
+        <v>12</v>
+      </c>
+      <c r="P114" s="2">
+        <v>48</v>
+      </c>
+      <c r="Q114" s="2">
+        <v>23</v>
+      </c>
+      <c r="R114" s="2">
+        <v>2</v>
+      </c>
+      <c r="S114" s="2">
+        <v>41</v>
+      </c>
+      <c r="T114" s="2">
+        <v>36</v>
+      </c>
+      <c r="U114" s="2">
+        <v>119</v>
+      </c>
+      <c r="V114" s="2">
+        <v>28</v>
+      </c>
+      <c r="W114" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23">
+      <c r="A115" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B115" s="2">
+        <v>663</v>
+      </c>
+      <c r="C115" s="2">
+        <v>19</v>
+      </c>
+      <c r="D115" s="2">
+        <v>16</v>
+      </c>
+      <c r="E115" s="2">
+        <v>0</v>
+      </c>
+      <c r="F115" s="2">
+        <v>27</v>
+      </c>
+      <c r="G115" s="2">
+        <v>34</v>
+      </c>
+      <c r="H115" s="2">
+        <v>18</v>
+      </c>
+      <c r="I115" s="2">
+        <v>45</v>
+      </c>
+      <c r="J115" s="2">
+        <v>13</v>
+      </c>
+      <c r="K115" s="2">
+        <v>32</v>
+      </c>
+      <c r="L115" s="2">
+        <v>10</v>
+      </c>
+      <c r="M115" s="2">
+        <v>37</v>
+      </c>
+      <c r="N115" s="2">
+        <v>84</v>
+      </c>
+      <c r="O115" s="2">
+        <v>19</v>
+      </c>
+      <c r="P115" s="2">
+        <v>35</v>
+      </c>
+      <c r="Q115" s="2">
+        <v>27</v>
+      </c>
+      <c r="R115" s="2">
+        <v>14</v>
+      </c>
+      <c r="S115" s="2">
+        <v>33</v>
+      </c>
+      <c r="T115" s="2">
+        <v>40</v>
+      </c>
+      <c r="U115" s="2">
+        <v>104</v>
+      </c>
+      <c r="V115" s="2">
         <v>26</v>
       </c>
-      <c r="C112" s="2">
-        <v>0</v>
-      </c>
-      <c r="D112" s="2">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2">
-        <v>1</v>
-      </c>
-      <c r="G112" s="2">
-        <v>0</v>
-      </c>
-      <c r="H112" s="2">
-        <v>0</v>
-      </c>
-      <c r="I112" s="2">
-        <v>0</v>
-      </c>
-      <c r="J112" s="2">
-        <v>0</v>
-      </c>
-      <c r="K112" s="2">
-        <v>0</v>
-      </c>
-      <c r="L112" s="2">
-        <v>0</v>
-      </c>
-      <c r="M112" s="2">
-        <v>0</v>
-      </c>
-      <c r="N112" s="2">
-        <v>22</v>
-      </c>
-      <c r="O112" s="2">
-        <v>0</v>
-      </c>
-      <c r="P112" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q112" s="2">
-        <v>0</v>
-      </c>
-      <c r="R112" s="2">
-        <v>0</v>
-      </c>
-      <c r="S112" s="2">
-        <v>1</v>
-      </c>
-      <c r="T112" s="2">
-        <v>0</v>
-      </c>
-      <c r="U112" s="2">
-        <v>2</v>
-      </c>
-      <c r="V112" s="2">
-        <v>0</v>
-      </c>
-      <c r="W112" s="2">
-        <v>0</v>
-      </c>
+      <c r="W115" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23">
+      <c r="A116" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B116" s="2">
+        <v>127</v>
+      </c>
+      <c r="C116" s="2">
+        <v>0</v>
+      </c>
+      <c r="D116" s="2">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2">
+        <v>0</v>
+      </c>
+      <c r="F116" s="2">
+        <v>5</v>
+      </c>
+      <c r="G116" s="2">
+        <v>5</v>
+      </c>
+      <c r="H116" s="2">
+        <v>8</v>
+      </c>
+      <c r="I116" s="2">
+        <v>13</v>
+      </c>
+      <c r="J116" s="2">
+        <v>1</v>
+      </c>
+      <c r="K116" s="2">
+        <v>0</v>
+      </c>
+      <c r="L116" s="2">
+        <v>2</v>
+      </c>
+      <c r="M116" s="2">
+        <v>15</v>
+      </c>
+      <c r="N116" s="2">
+        <v>25</v>
+      </c>
+      <c r="O116" s="2">
+        <v>1</v>
+      </c>
+      <c r="P116" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q116" s="2">
+        <v>0</v>
+      </c>
+      <c r="R116" s="2">
+        <v>1</v>
+      </c>
+      <c r="S116" s="2">
+        <v>4</v>
+      </c>
+      <c r="T116" s="2">
+        <v>8</v>
+      </c>
+      <c r="U116" s="2">
+        <v>30</v>
+      </c>
+      <c r="V116" s="2">
+        <v>9</v>
+      </c>
+      <c r="W116" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23">
+      <c r="B117" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8472,15 +8763,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8776,7 +9067,7 @@
         <v>43936</v>
       </c>
       <c r="B37" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -8880,7 +9171,7 @@
         <v>43949</v>
       </c>
       <c r="B50" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -8888,7 +9179,7 @@
         <v>43950</v>
       </c>
       <c r="B51" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -8904,7 +9195,7 @@
         <v>43952</v>
       </c>
       <c r="B53" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -8920,7 +9211,7 @@
         <v>43954</v>
       </c>
       <c r="B55" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -8928,7 +9219,7 @@
         <v>43955</v>
       </c>
       <c r="B56" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -8936,7 +9227,7 @@
         <v>43956</v>
       </c>
       <c r="B57" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -8960,7 +9251,7 @@
         <v>43959</v>
       </c>
       <c r="B60" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -8968,7 +9259,7 @@
         <v>43960</v>
       </c>
       <c r="B61" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -8976,7 +9267,7 @@
         <v>43961</v>
       </c>
       <c r="B62" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -8984,7 +9275,7 @@
         <v>43962</v>
       </c>
       <c r="B63" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -8992,7 +9283,7 @@
         <v>43963</v>
       </c>
       <c r="B64" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -9000,7 +9291,7 @@
         <v>43964</v>
       </c>
       <c r="B65" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -9008,7 +9299,7 @@
         <v>43965</v>
       </c>
       <c r="B66" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -9016,7 +9307,7 @@
         <v>43966</v>
       </c>
       <c r="B67" s="2">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -9024,7 +9315,7 @@
         <v>43967</v>
       </c>
       <c r="B68" s="2">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -9032,7 +9323,7 @@
         <v>43968</v>
       </c>
       <c r="B69" s="2">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -9040,7 +9331,7 @@
         <v>43969</v>
       </c>
       <c r="B70" s="2">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -9048,7 +9339,7 @@
         <v>43970</v>
       </c>
       <c r="B71" s="2">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -9056,7 +9347,7 @@
         <v>43971</v>
       </c>
       <c r="B72" s="2">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -9064,7 +9355,7 @@
         <v>43972</v>
       </c>
       <c r="B73" s="2">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -9072,7 +9363,7 @@
         <v>43973</v>
       </c>
       <c r="B74" s="2">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -9080,16 +9371,51 @@
         <v>43974</v>
       </c>
       <c r="B75" s="2">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B76" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B77" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B78" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B79" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B76" s="2">
-        <v>20</v>
-      </c>
+      <c r="B80" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9098,13 +9424,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -9303,7 +9629,7 @@
         <v>43919</v>
       </c>
       <c r="B25" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -9311,7 +9637,7 @@
         <v>43920</v>
       </c>
       <c r="B26" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -9335,7 +9661,7 @@
         <v>43923</v>
       </c>
       <c r="B29" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -9343,7 +9669,7 @@
         <v>43924</v>
       </c>
       <c r="B30" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -9423,7 +9749,7 @@
         <v>43934</v>
       </c>
       <c r="B40" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -9439,7 +9765,7 @@
         <v>43936</v>
       </c>
       <c r="B42" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -9447,7 +9773,7 @@
         <v>43937</v>
       </c>
       <c r="B43" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -9487,7 +9813,7 @@
         <v>43942</v>
       </c>
       <c r="B48" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -9503,7 +9829,7 @@
         <v>43944</v>
       </c>
       <c r="B50" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -9511,7 +9837,7 @@
         <v>43945</v>
       </c>
       <c r="B51" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -9599,7 +9925,7 @@
         <v>43956</v>
       </c>
       <c r="B62" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -9623,7 +9949,7 @@
         <v>43959</v>
       </c>
       <c r="B65" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -9703,7 +10029,7 @@
         <v>43969</v>
       </c>
       <c r="B75" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -9711,7 +10037,7 @@
         <v>43970</v>
       </c>
       <c r="B76" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -9719,7 +10045,7 @@
         <v>43971</v>
       </c>
       <c r="B77" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -9727,7 +10053,7 @@
         <v>43972</v>
       </c>
       <c r="B78" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -9735,7 +10061,7 @@
         <v>43973</v>
       </c>
       <c r="B79" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -9743,7 +10069,7 @@
         <v>43974</v>
       </c>
       <c r="B80" s="2">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -9751,8 +10077,43 @@
         <v>43975</v>
       </c>
       <c r="B81" s="2">
-        <v>3</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B82" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B83" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B84" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B85" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="B86" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9761,13 +10122,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -9791,10 +10152,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="C2" s="2">
-        <v>90.222175598144531</v>
+        <v>113.40425872802734</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -9808,16 +10169,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1124</v>
+        <v>1174</v>
       </c>
       <c r="C3" s="2">
-        <v>390.3238525390625</v>
+        <v>407.68701171875</v>
       </c>
       <c r="D3" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -9825,16 +10186,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2">
-        <v>115.60499572753906</v>
+        <v>117.28043365478516</v>
       </c>
       <c r="D4" s="2">
         <v>5</v>
       </c>
       <c r="E4" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9842,16 +10203,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1123</v>
+        <v>1202</v>
       </c>
       <c r="C5" s="2">
-        <v>390.76907348632813</v>
+        <v>418.25863647460938</v>
       </c>
       <c r="D5" s="2">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -9859,16 +10220,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>653</v>
+        <v>723</v>
       </c>
       <c r="C6" s="2">
-        <v>195.59799194335938</v>
+        <v>216.56562805175781</v>
       </c>
       <c r="D6" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9876,16 +10237,16 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>628</v>
+        <v>678</v>
       </c>
       <c r="C7" s="2">
-        <v>480.08563232421875</v>
+        <v>518.30902099609375</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -9893,16 +10254,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1294</v>
+        <v>1449</v>
       </c>
       <c r="C8" s="2">
-        <v>355.88656616210938</v>
+        <v>398.51596069335938</v>
       </c>
       <c r="D8" s="2">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -9910,16 +10271,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>279</v>
+        <v>326</v>
       </c>
       <c r="C9" s="2">
-        <v>113.67062377929688</v>
+        <v>132.81944274902344</v>
       </c>
       <c r="D9" s="2">
         <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -9927,16 +10288,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>718</v>
+        <v>797</v>
       </c>
       <c r="C10" s="2">
-        <v>356.38238525390625</v>
+        <v>395.5943603515625</v>
       </c>
       <c r="D10" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9944,16 +10305,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>360</v>
+        <v>388</v>
       </c>
       <c r="C11" s="2">
-        <v>143.94645690917969</v>
+        <v>155.14228820800781</v>
       </c>
       <c r="D11" s="2">
         <v>37</v>
       </c>
       <c r="E11" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -9961,16 +10322,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1482</v>
+        <v>1623</v>
       </c>
       <c r="C12" s="2">
-        <v>107.56067657470703</v>
+        <v>117.79418182373047</v>
       </c>
       <c r="D12" s="2">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -9978,16 +10339,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>11211</v>
+        <v>11652</v>
       </c>
       <c r="C13" s="2">
-        <v>471.62884521484375</v>
+        <v>490.1810302734375</v>
       </c>
       <c r="D13" s="2">
-        <v>752</v>
+        <v>778</v>
       </c>
       <c r="E13" s="2">
-        <v>1936</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -9995,16 +10356,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1563</v>
+        <v>1612</v>
       </c>
       <c r="C14" s="2">
-        <v>525.3074951171875</v>
+        <v>541.77587890625</v>
       </c>
       <c r="D14" s="2">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E14" s="2">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10012,16 +10373,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>1662</v>
+        <v>1803</v>
       </c>
       <c r="C15" s="2">
-        <v>433.13623046875</v>
+        <v>469.8824462890625</v>
       </c>
       <c r="D15" s="2">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10029,16 +10390,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>403</v>
+        <v>459</v>
       </c>
       <c r="C16" s="2">
-        <v>142.69830322265625</v>
+        <v>162.52735900878906</v>
       </c>
       <c r="D16" s="2">
         <v>20</v>
       </c>
       <c r="E16" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10046,16 +10407,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="C17" s="2">
-        <v>170.75396728515625</v>
+        <v>177.37803649902344</v>
       </c>
       <c r="D17" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -10063,16 +10424,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>572</v>
+        <v>673</v>
       </c>
       <c r="C18" s="2">
-        <v>233.13919067382813</v>
+        <v>274.30535888671875</v>
       </c>
       <c r="D18" s="2">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E18" s="2">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -10080,16 +10441,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1118</v>
+        <v>1231</v>
       </c>
       <c r="C19" s="2">
-        <v>405.30007934570313</v>
+        <v>446.26510620117188</v>
       </c>
       <c r="D19" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -10097,16 +10458,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>5050</v>
+        <v>5480</v>
       </c>
       <c r="C20" s="2">
-        <v>292.60418701171875</v>
+        <v>317.51898193359375</v>
       </c>
       <c r="D20" s="2">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="E20" s="2">
-        <v>474</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10114,16 +10475,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1639</v>
+        <v>1750</v>
       </c>
       <c r="C21" s="2">
-        <v>537.7208251953125</v>
+        <v>574.1375732421875</v>
       </c>
       <c r="D21" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E21" s="2">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10131,17 +10492,23 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>1903</v>
+        <v>1974</v>
       </c>
       <c r="C22" s="2">
-        <v>408.8121337890625</v>
+        <v>424.064697265625</v>
       </c>
       <c r="D22" s="2">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E22" s="2">
-        <v>165</v>
-      </c>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10152,11 +10519,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -10177,13 +10542,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>13773</v>
+        <v>14622</v>
       </c>
       <c r="C2" s="2">
-        <v>1434</v>
+        <v>1504</v>
       </c>
       <c r="D2" s="2">
-        <v>2208</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -10191,13 +10556,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>19683</v>
+        <v>21101</v>
       </c>
       <c r="C3" s="2">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="D3" s="2">
-        <v>1790</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -10205,7 +10570,7 @@
         <v>36</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -10223,11 +10588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -10248,7 +10611,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C2" s="2">
         <v>4</v>
@@ -10262,10 +10625,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>386</v>
+        <v>424</v>
       </c>
       <c r="C3" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -10276,10 +10639,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>3006</v>
+        <v>3268</v>
       </c>
       <c r="C4" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -10290,10 +10653,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>3926</v>
+        <v>4264</v>
       </c>
       <c r="C5" s="2">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2">
         <v>12</v>
@@ -10304,13 +10667,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>4793</v>
+        <v>5182</v>
       </c>
       <c r="C6" s="2">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D6" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -10318,13 +10681,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>6008</v>
+        <v>6446</v>
       </c>
       <c r="C7" s="2">
-        <v>507</v>
+        <v>534</v>
       </c>
       <c r="D7" s="2">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -10332,13 +10695,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>4071</v>
+        <v>4345</v>
       </c>
       <c r="C8" s="2">
-        <v>582</v>
+        <v>605</v>
       </c>
       <c r="D8" s="2">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -10346,13 +10709,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>3800</v>
+        <v>3972</v>
       </c>
       <c r="C9" s="2">
-        <v>372</v>
+        <v>398</v>
       </c>
       <c r="D9" s="2">
-        <v>885</v>
+        <v>934</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -10360,13 +10723,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>4702</v>
+        <v>4935</v>
       </c>
       <c r="C10" s="2">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2">
-        <v>1638</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -10374,13 +10737,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>2600</v>
+        <v>2711</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1007</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -10388,7 +10751,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -10408,7 +10771,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>